<commit_message>
Updated 3d printing instructions
</commit_message>
<xml_diff>
--- a/Instructions/3D Printing Instructions.xlsx
+++ b/Instructions/3D Printing Instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\AI-Case-Sorter-CS7.2\Instructions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2193DB38-287C-46AD-82E5-3C2772E11606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88ACE06F-0EC2-4F25-BC1A-26FBFD1E1ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{65265D6A-040B-4E5E-B90C-A65C0E71D1E1}"/>
+    <workbookView xWindow="29580" yWindow="2625" windowWidth="26475" windowHeight="11565" xr2:uid="{65265D6A-040B-4E5E-B90C-A65C0E71D1E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -747,9 +747,9 @@
   </sheetPr>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1:E1048576"/>
+      <selection pane="topRight" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,10 +878,10 @@
         <v>0.16</v>
       </c>
       <c r="H3" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I3" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>7</v>
@@ -894,7 +894,7 @@
       </c>
       <c r="N3"/>
     </row>
-    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -914,13 +914,13 @@
         <v>45</v>
       </c>
       <c r="G4" s="4">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="H4" s="4">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="I4" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>7</v>
@@ -956,7 +956,7 @@
         <v>0.2</v>
       </c>
       <c r="H5" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I5" s="4">
         <v>3</v>
@@ -995,7 +995,7 @@
         <v>0.2</v>
       </c>
       <c r="H6" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I6" s="4">
         <v>3</v>
@@ -1034,7 +1034,7 @@
         <v>0.2</v>
       </c>
       <c r="H7" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I7" s="4">
         <v>3</v>
@@ -1076,7 +1076,7 @@
         <v>0.2</v>
       </c>
       <c r="H8" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I8" s="4">
         <v>3</v>
@@ -1115,7 +1115,7 @@
         <v>0.2</v>
       </c>
       <c r="H9" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I9" s="4">
         <v>3</v>
@@ -1157,7 +1157,7 @@
         <v>0.16</v>
       </c>
       <c r="H10" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I10" s="4">
         <v>3</v>
@@ -1196,7 +1196,7 @@
         <v>0.2</v>
       </c>
       <c r="H11" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I11" s="4">
         <v>3</v>
@@ -1235,7 +1235,7 @@
         <v>0.2</v>
       </c>
       <c r="H12" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I12" s="4">
         <v>3</v>
@@ -1277,7 +1277,7 @@
         <v>0.2</v>
       </c>
       <c r="H13" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I13" s="4">
         <v>3</v>
@@ -1316,7 +1316,7 @@
         <v>0.2</v>
       </c>
       <c r="H14" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I14" s="4">
         <v>3</v>
@@ -1355,7 +1355,7 @@
         <v>0.2</v>
       </c>
       <c r="H15" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I15" s="4">
         <v>3</v>
@@ -1397,7 +1397,7 @@
         <v>0.2</v>
       </c>
       <c r="H16" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I16" s="4">
         <v>3</v>
@@ -1436,7 +1436,7 @@
         <v>0.2</v>
       </c>
       <c r="H17" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I17" s="4">
         <v>3</v>
@@ -1475,7 +1475,7 @@
         <v>0.2</v>
       </c>
       <c r="H18" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I18" s="4">
         <v>3</v>
@@ -1514,7 +1514,7 @@
         <v>0.2</v>
       </c>
       <c r="H19" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I19" s="4">
         <v>3</v>
@@ -1631,7 +1631,7 @@
         <v>0.2</v>
       </c>
       <c r="H22" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I22" s="4">
         <v>3</v>
@@ -1670,7 +1670,7 @@
         <v>0.2</v>
       </c>
       <c r="H23" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I23" s="4">
         <v>3</v>
@@ -1748,7 +1748,7 @@
         <v>0.2</v>
       </c>
       <c r="H25" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I25" s="4">
         <v>3</v>
@@ -1787,7 +1787,7 @@
         <v>0.2</v>
       </c>
       <c r="H26" s="4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I26" s="4">
         <v>3</v>

</xml_diff>